<commit_message>
docs. update FSNM201-exercise-file by yezi
</commit_message>
<xml_diff>
--- a/0-产品推广数据监测表-20170829.xlsx
+++ b/0-产品推广数据监测表-20170829.xlsx
@@ -91,29 +91,6 @@
     <t>新媒体人必会的傻瓜式爬虫工具：上手 Web Scraper 的 5 个步骤</t>
   </si>
   <si>
-    <t>Day5文章阅读量</t>
-    <rPh sb="4" eb="5">
-      <t>wen zhang</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>yue du</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>liang</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Day5知乎排名</t>
-    <rPh sb="4" eb="5">
-      <t>zhi hu</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>pai ming</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.jianshu.com/p/da44178a5813</t>
   </si>
   <si>
@@ -151,32 +128,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Day5页面浏览量</t>
-    <rPh sb="4" eb="5">
-      <t>ye mian</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>liu lan</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>liang</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Day5注册转化次数</t>
-    <rPh sb="4" eb="5">
-      <t>zhu ce</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>zhuan hua</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ci shu</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>阅读-注册转化率</t>
     <rPh sb="0" eb="1">
       <t>yue du</t>
@@ -237,6 +188,61 @@
     </rPh>
     <rPh sb="15" eb="16">
       <t>shu ju</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>累计5天文章阅读量</t>
+    <rPh sb="0" eb="1">
+      <t>lei ji</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>tian</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>wen zhang</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>yue du</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>liang</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>累计5天知乎排名</t>
+    <rPh sb="4" eb="5">
+      <t>zhi hu</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>pai ming</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>累计5天页面浏览量</t>
+    <rPh sb="4" eb="5">
+      <t>ye mian</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>liu lan</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>liang</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>累计5天注册转化次数</t>
+    <rPh sb="4" eb="5">
+      <t>zhu ce</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>zhuan hua</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ci shu</t>
     </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -886,7 +892,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,10 +902,10 @@
     <col min="3" max="3" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.1640625" style="16" customWidth="1"/>
     <col min="11" max="11" width="16.5" style="16" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="10.83203125" style="2"/>
@@ -922,22 +928,22 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -948,7 +954,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>7</v>
@@ -982,22 +988,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" s="9">
         <v>1115</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H3" s="9">
         <v>115</v>
@@ -1286,7 +1292,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -1297,7 +1303,7 @@
         <v>2171</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H22" s="18">
         <f>SUM(H2:H21)</f>
@@ -1318,10 +1324,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revert "Revert "docs: update-data-excel-link""
This reverts commit d01501a46ee1554601cafc5101af1acf70042830.
</commit_message>
<xml_diff>
--- a/0-产品推广数据监测表-20170829.xlsx
+++ b/0-产品推广数据监测表-20170829.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -892,7 +895,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>